<commit_message>
Fix elective scheduling and legend rendering for 'Whole' timetables by normalizing section IDs, adding fallback ID matching, and adding tests
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_post_mid_timetable.xlsx
+++ b/backend/output_timetables/sem1_CSE_post_mid_timetable.xlsx
@@ -11,6 +11,11 @@
     <sheet name="Section_B" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Verification_A" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Verification_B" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="LTPSC_Compliance" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Executive_Summary" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Course_Summary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Distribution_Logic" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="All_Courses_Overview" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -481,17 +486,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>MA162</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>DS161</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -508,22 +513,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>EC161</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>MA161</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -572,27 +577,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>CS161 (Lab)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CS161 (Lab)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>DS161</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -604,14 +609,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>CS161 (Lab)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CS161 (Lab)</t>
-        </is>
-      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>Free</t>
@@ -624,7 +629,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>ELECTIVE_B1 (Tutorial)</t>
         </is>
       </c>
     </row>
@@ -636,27 +641,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>HS161</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>EC161 (Lab)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>EC161</t>
         </is>
       </c>
     </row>
@@ -683,12 +688,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>EC161 (Lab)</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
     </row>
@@ -756,12 +761,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -771,7 +776,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -788,22 +793,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>MA161</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>DS161</t>
         </is>
       </c>
     </row>
@@ -847,27 +852,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>CS161 (Lab)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>CS161</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>CS161 (Lab)</t>
         </is>
       </c>
     </row>
@@ -884,7 +889,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>EC161 (Lab)</t>
+          <t>CS161 (Lab)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -899,7 +904,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>CS161 (Lab)</t>
+          <t>ELECTIVE_B1 (Tutorial)</t>
         </is>
       </c>
     </row>
@@ -911,27 +916,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>DS161</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>EC161 (Lab)</t>
         </is>
       </c>
     </row>
@@ -963,7 +968,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161 (Lab)</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1051,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>–</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1083,17 +1088,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>**CS161**</t>
+          <t>**MA162**</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>introduction to cyber security</t>
+          <t>Probability</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Chinmayananda</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1108,7 +1113,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2/1</t>
+          <t>0/0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1130,22 +1135,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>**HS161**</t>
+          <t>**CS161**</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>English Language</t>
+          <t>introduction to cyber security</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Rajesh N S</t>
+          <t>Girish Revadigar</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3-0-0-0-3</t>
+          <t>2-0-0-0-2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1155,7 +1160,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0/0</t>
+          <t>2/1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -1165,7 +1170,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Partial</t>
+          <t>Complete</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1177,22 +1182,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>**MA162**</t>
+          <t>**MA161**</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Chinmayananda</t>
+          <t>Ramesh Athe</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>3-0-2-0-2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1212,7 +1217,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Partial</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1224,17 +1229,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>**MA161**</t>
+          <t>**EC161**</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Digital Design</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ramesh Athe</t>
+          <t>Prakash Pawar</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1249,7 +1254,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0/0</t>
+          <t>2/1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1271,22 +1276,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>**EC161**</t>
+          <t>**DS161**</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>Introduction to DATA science and artificial intelligence</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Prakash Pawar</t>
+          <t>Girish Revadigar</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3-0-2-0-2</t>
+          <t>2-0-0-0-2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1296,7 +1301,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2/1</t>
+          <t>0/0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1306,7 +1311,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Partial</t>
+          <t>Complete</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1318,22 +1323,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>**DS161**</t>
+          <t>**HS161**</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Introduction to DATA science and artificial intelligence</t>
+          <t>English Language</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Rajesh N S</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>3-0-0-0-3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1353,7 +1358,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Partial</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1385,7 +1390,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lectures: 13</t>
+          <t>Lectures: 14</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1488,7 +1493,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>–</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1572,17 +1577,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>**MA162**</t>
+          <t>**DS161**</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Introduction to DATA science and artificial intelligence</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Chinmayananda</t>
+          <t>Girish Revadigar</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1619,12 +1624,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>**DS161**</t>
+          <t>**CS161**</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Introduction to DATA science and artificial intelligence</t>
+          <t>introduction to cyber security</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1644,7 +1649,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0/0</t>
+          <t>2/1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1666,17 +1671,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>**MA161**</t>
+          <t>**EC161**</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Digital Design</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ramesh Athe</t>
+          <t>Prakash Pawar</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1691,7 +1696,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0/0</t>
+          <t>2/1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1713,17 +1718,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>**EC161**</t>
+          <t>**MA161**</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Prakash Pawar</t>
+          <t>Ramesh Athe</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1738,7 +1743,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2/1</t>
+          <t>0/0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1760,17 +1765,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>**CS161**</t>
+          <t>**MA162**</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>introduction to cyber security</t>
+          <t>Probability</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Chinmayananda</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1785,7 +1790,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2/1</t>
+          <t>0/0</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1827,7 +1832,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lectures: 13</t>
+          <t>Lectures: 14</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1848,6 +1853,3883 @@
       <c r="I9" t="inlineStr">
         <is>
           <t>--</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Required LTPSC</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Required (L/T/P)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Section A (L/T/P)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Section B (L/T/P)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lectures Status</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Tutorials Status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Labs Status</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Overall Compliance</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>introduction to cyber security</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2/0/2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2/0/2</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>[OK] FULLY COMPLIANT</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Meets requirements</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Introduction to DATA science and artificial intelligence</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>[OK] FULLY COMPLIANT</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Meets requirements</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3-0-2-0-2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3/0/2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2/0/2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2/0/2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[FAIL]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>[WARN] PARTIAL</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Check scheduling</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3-0-0-0-3</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3/0/0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2/1/0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2/1/0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[FAIL]</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>[WARN] PARTIAL</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Check scheduling</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>English Language</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3-0-0-0-3</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3/0/0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>[FAIL]</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>[WARN] PARTIAL</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Check scheduling</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3-0-2-0-2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3/0/2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>[FAIL]</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>[FAIL]</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>[WARN] PARTIAL</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Check scheduling</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2/0/0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>[OK]</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>[OK] FULLY COMPLIANT</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Meets requirements</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Details</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Basic Information</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Branch: CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Basic Information</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Generation Date</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-12-13 16:20</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Timetable generation timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Course Statistics</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Total Courses</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Core: 5, Elective: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LTPSC Compliance</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Compliance Rate</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>42.9%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3/7 courses fully compliant</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Room Utilization</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rooms Used</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0/35</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Utilization: 0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Schedule Density</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Time Slot Utilization</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>54.3%</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>A: 54.3%, B: 54.3%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Quality Assessment</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Overall Quality</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[WARN] NEEDS REVIEW</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Score: 57.4/100</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Schedule Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Branch</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Credits</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>LTPSC</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lectures/Week</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Tutorials/Week</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Practicals/Week</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Half Semester</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Post mid-sem</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Inclusion Reasoning</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Problem Solving</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>3-0-2-0-4</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Sunil P V, Sunil C K, Animesh Roy</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Half Semester = No, Post mid-sem = No (pre-mid only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>English Language</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>3-0-0-0-3</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Half Semester = No, Post mid-sem = No (pre-mid only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Computational musicology for hindustani music</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1-0-0-0-1</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Chandrika Kamat</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Half Semester = No, Post mid-sem = No (pre-mid only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1-0-0-0-1</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Half Semester = No, Post mid-sem = No (pre-mid only)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Chinmayananda</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Half Semester = Yes (scheduled in both pre-mid and post-mid)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>3-0-2-0-2</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Prakash Pawar</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Half Semester = Yes (scheduled in both pre-mid and post-mid)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>introduction to cyber security</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Girish Revadigar</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Half Semester = Yes (scheduled in both pre-mid and post-mid)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Ramesh Athe</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Half Semester = Yes (scheduled in both pre-mid and post-mid)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Introduction to DS and AI</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Girish Revadigar</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Half Semester = Yes (scheduled in both pre-mid and post-mid)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Credits</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Post mid-sem</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Scheduled In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Logic Applied</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>In Pre-Mid</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>In Post-Mid</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Branch</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Introduction to data science and artifical inteligance</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='Yes' -&gt; Post-Mid Only</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='Yes' -&gt; Post-Mid Only</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Problem Solving</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>4-credit + Post mid-sem='No' -&gt; BOTH Pre-Mid &amp; Post-Mid</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>English Language</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3-credit + Post mid-sem='No' -&gt; BOTH Pre-Mid &amp; Post-Mid</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Introduction to quantam Physics</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Linux for Engineers</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Fundamentals of Computing</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>introduction to cyber security</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Post-Mid Only</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='Yes' -&gt; Post-Mid Only</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Computational musicology for hindustani music</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1-credit + Post mid-sem='No' -&gt; BOTH Pre-Mid &amp; Post-Mid</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Kannada Kali-Nali</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Leveraging IT for Better Life</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Basics of Design</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>1-credit + Post mid-sem='No' -&gt; BOTH Pre-Mid &amp; Post-Mid</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='Yes' -&gt; Post-Mid Only</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Introduction to DS and AI</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='Yes' -&gt; Post-Mid Only</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='Yes' -&gt; Post-Mid Only</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Introduction to DATA science and artificial intelligence</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='Yes' -&gt; Post-Mid Only</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2-credit + Post mid-sem='No' -&gt; Pre-Mid Only</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Problem Solving</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Both (non-2-credit with Post mid-sem='No')</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>4-credit + Post mid-sem='No' -&gt; BOTH Pre-Mid &amp; Post-Mid</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Credits</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Branch</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Schedule Type</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Post mid-sem</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Half Semester</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Problem Solving</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Sunil P V, Sunil C K, Animesh Roy</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>English Language</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Computational musicology for hindustani music</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Chandrika Kamat</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Ramesh Athe</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Introduction to data science and artifical inteligance</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Abdul Wahid</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Introduction to quantam Physics</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Ravishankar, Vivekraj</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Linux for Engineers</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Vivekraj</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Fundamentals of Computing</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Mallikarjun Kande</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Kannada Kali-Nali</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Anand B</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Leveraging IT for Better Life</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Basics of Design</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Sandesh Phalke</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Chinmayananda</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Pre-Mid</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Prakash Pawar</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Problem Solving</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Sunil P V, Sunil C K, Animesh Roy</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>English Language</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Computational musicology for hindustani music</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Chandrika Kamat</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Chinmayananda</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Prakash Pawar</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>introduction to cyber security</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Girish Revadigar</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Ramesh Athe</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Introduction to DS and AI</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Post-Mid</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Girish Revadigar</t>
         </is>
       </c>
     </row>

</xml_diff>